<commit_message>
update glossary excel file
</commit_message>
<xml_diff>
--- a/docs/glossary.xlsx
+++ b/docs/glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oleksandrlevchuk/Desktop/CommDocs/Comm-Docs-Project-Alx-Tony/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4486CA3-B088-954C-9C6E-53EC6AB010BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27023672-23CA-FE47-BAB9-6A3B1C1CF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="23620" windowHeight="14960" xr2:uid="{AD715D2C-FB16-AB45-8476-CB247902B4F8}"/>
+    <workbookView xWindow="5180" yWindow="1780" windowWidth="23620" windowHeight="14960" xr2:uid="{AD715D2C-FB16-AB45-8476-CB247902B4F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Term</t>
   </si>
@@ -47,7 +47,65 @@
     <t>**brew**</t>
   </si>
   <si>
-    <t>Brew command is a command-line tool for macOS that allows users to install and manage software packages.</t>
+    <t>**git config**</t>
+  </si>
+  <si>
+    <t>Command-line tool used to set and manage Git configuration options at different levels (system, user, and repository)</t>
+  </si>
+  <si>
+    <t>**git add**</t>
+  </si>
+  <si>
+    <t>**git commit**</t>
+  </si>
+  <si>
+    <t>**repository**</t>
+  </si>
+  <si>
+    <t>**git push**</t>
+  </si>
+  <si>
+    <t>**git pull**</t>
+  </si>
+  <si>
+    <t>**git clone**</t>
+  </si>
+  <si>
+    <t>**branch**</t>
+  </si>
+  <si>
+    <t>**HEAD**</t>
+  </si>
+  <si>
+    <t>A central location where Git version control system stores all the data related to a project, including the entire history of changes made to the project over time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`git clone` is a command used to create a copy of a remote Git repository onto a local machine, allowing developers to work on the codebase without directly modifying the original repository.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`git pull` is a command used in Git version control system to merge changes from a remote repository to a local repository, ensuring that the local repository is up to date with the remote repository
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`git push` is a command used in Git version control system to upload the local repository changes to a remote repository, typically hosted on GitHub
+</t>
+  </si>
+  <si>
+    <t>`git commit` is a command used in Git version control system to save the changes made to a file or a set of files along with a descriptive message that explains the changes</t>
+  </si>
+  <si>
+    <t>`git add` is a Git command used to stage changes made to files in a repository, preparing them to be committed to the repository's history</t>
+  </si>
+  <si>
+    <t>`brew` command is a command-line tool for macOS that allows users to install and manage software packages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Git version control system, a branch is a parallel version of the main codebase that allows developers to work on new features or modifications without directly affecting the main codebase until the changes are ready to be merged
+</t>
+  </si>
+  <si>
+    <t>In Git, HEAD is like a bookmark that points to the current version of your code that you're working on. Whenever you make changes and commit them, HEAD gets updated to point to the latest commit</t>
   </si>
 </sst>
 </file>
@@ -71,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -94,14 +152,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB35FB46-E4C3-F940-AB18-D5535791289C}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,37 +511,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>